<commit_message>
Guion 2 Final - Guion 3 Original Autor
Archivos finales de Guion 2 revisados y aprobados con corrección de
estilo, solicitud gráfica modificada por solicitud de graficador.
Archivo de guion 3 y recursos original de autor, en revisión. Archivos
borrados de la carpeta visuales. Muchas gracias.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion02/EsqueletoGuión_CN_10_02_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion02/EsqueletoGuión_CN_10_02_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729" activeTab="1"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -1610,7 +1610,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1693,8 +1693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2450,7 +2450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Versión de revisión guion 3
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion02/EsqueletoGuión_CN_10_02_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion02/EsqueletoGuión_CN_10_02_CO.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729" activeTab="4"/>
@@ -18,14 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'CUADERNO DEL PROFESOR'!$A$1:$C$23</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1348,9 +1341,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1681,11 +1671,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2022,11 +2007,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2149,11 +2129,6 @@
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2438,11 +2413,6 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="71" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2450,7 +2420,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2459,7 +2431,7 @@
     <col min="3" max="3" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="61.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="17.85546875" style="3" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="17.85546875" style="3" customWidth="1"/>
     <col min="8" max="8" width="100.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.5703125" style="5" customWidth="1"/>
   </cols>
@@ -3966,10 +3938,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>